<commit_message>
problemas resueltos hasta el 14
</commit_message>
<xml_diff>
--- a/INTRODUCCIÓN A LA INFORMÁTICA/Excel/Ejercicios_Resueltos/EJERCICIO 12_UNIDAD 1.xlsx
+++ b/INTRODUCCIÓN A LA INFORMÁTICA/Excel/Ejercicios_Resueltos/EJERCICIO 12_UNIDAD 1.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UTN PACHECO\GUIA CURSO DE INGRESO 2024_bak\Resueltos_Guias_Repaso_TUP_2024_2025\INTRODUCCIÓN A LA INFORMÁTICA\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UTN PACHECO\GUIA CURSO DE INGRESO 2024_bak\Resueltos_Guias_Repaso_TUP_2024_2025\INTRODUCCIÓN A LA INFORMÁTICA\Excel\Ejercicios_Resueltos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{94EE8759-8F84-4D1C-BAE9-3A4D3BED3A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{2E4CDFBC-1FC1-433A-8447-A6B8B20481D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="25815" yWindow="2415" windowWidth="11940" windowHeight="12765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -237,109 +234,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val=".xlsx]EJERCICIO-1"/>
-      <sheetName val=".xlsx]EJERCICIO-2"/>
-      <sheetName val=".xlsx]EJERCICIO-3"/>
-      <sheetName val=".xlsx]EJERCICIO-4"/>
-      <sheetName val=".xlsx]EJERCICIO-5"/>
-      <sheetName val=".xlsx]EJERCICIO-6"/>
-      <sheetName val=".xlsx]EJERCICIO-7"/>
-      <sheetName val=".xlsx]EJERCICIO-8"/>
-      <sheetName val=".xlsx]EJERCICIO-9"/>
-      <sheetName val=".xlsx]EJERCICIO-10"/>
-      <sheetName val=".xlsx]EJERCICIO-11"/>
-      <sheetName val=".xlsx]RESUMEN-EJERCICIO-11"/>
-      <sheetName val=".xlsx]EJERCICIO-12"/>
-      <sheetName val=".xlsx]Resumen-ejercicio12"/>
-      <sheetName val=".xlsx]EJERCICIO-13"/>
-      <sheetName val=".xlsx]EJERCICIO-14"/>
-      <sheetName val=".xlsx]Datos-ejercicio14"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12">
-        <row r="2">
-          <cell r="I2" t="str">
-            <v>MP / CRÉDITO</v>
-          </cell>
-          <cell r="L2" t="str">
-            <v>Pan lactal</v>
-          </cell>
-          <cell r="M2">
-            <v>1800</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="I3" t="str">
-            <v>EFECTIVO</v>
-          </cell>
-          <cell r="L3" t="str">
-            <v>Galletas</v>
-          </cell>
-          <cell r="M3">
-            <v>600</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="L4" t="str">
-            <v>Pan rallado</v>
-          </cell>
-          <cell r="M4">
-            <v>850</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="L5" t="str">
-            <v>Budín marmolado</v>
-          </cell>
-          <cell r="M5">
-            <v>1300</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="L6" t="str">
-            <v>Pan de pebete</v>
-          </cell>
-          <cell r="M6">
-            <v>150</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="L7" t="str">
-            <v>Prepizzas</v>
-          </cell>
-          <cell r="M7">
-            <v>900</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -607,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,15 +574,15 @@
         <v>11</v>
       </c>
       <c r="J2" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!L2:L51,"MERCADO PAGO",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+        <f>SUMIF(E10:E34,"MERCADO PAGO",F10:F34)</f>
+        <v>136027.5</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M2" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Pan lactal",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+      <c r="M2" s="8">
+        <f>SUMIF($B$2:$B$51,"Pan lactal",$F$10:$F$59)</f>
+        <v>4455</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -714,14 +608,14 @@
         <v>10</v>
       </c>
       <c r="J3" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!L2:L51,"TARJETA DE CRÉDITO",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+        <f>SUMIF(E10:E34,"TARJETA DE CRÉDITO",F10:F34)</f>
+        <v>61635</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Galletas",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
+      <c r="M3" s="8">
+        <f>SUMIF($B$2:$B$51,"Galletas",$F$10:$F$59)</f>
         <v>0</v>
       </c>
     </row>
@@ -739,15 +633,15 @@
         <f>COUNTIF(E10:E34,"TARJETA DE DEBITO")</f>
         <v>2</v>
       </c>
-      <c r="J4" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!L2:L51,"TARJETA DE DEBITO",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+      <c r="J4" s="12" t="e">
+        <f>SUMIF(E10:E34,"TARJETA DE DEBITO",F10:F34)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Pan rallado",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
+      <c r="M4" s="8">
+        <f>SUMIF($B$2:$B$51,"Pan ralladoo",$F$10:$F$59)</f>
         <v>0</v>
       </c>
     </row>
@@ -766,15 +660,15 @@
         <v>9</v>
       </c>
       <c r="J5" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!L2:L51,"EFECTIVO",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+        <f>SUMIF(E10:E34,"EFECTIVO",F10:F34)</f>
+        <v>48015</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Budín marmolado",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+      <c r="M5" s="8">
+        <f>SUMIF($B$2:$B$51,"Budín marmolado",$F$10:$F$59)</f>
+        <v>23490</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,9 +681,9 @@
       <c r="L6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Pan de pebete",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+      <c r="M6" s="8">
+        <f>SUMIF($B$2:$B$51,"Pan de pebete",$F$10:$F$59)</f>
+        <v>17010</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -802,25 +696,25 @@
       <c r="H7" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="12" t="e">
-        <f>AVERAGE('[1].xlsx]EJERCICIO-12'!T2:T7)</f>
-        <v>#DIV/0!</v>
+      <c r="I7" s="12">
+        <f>AVERAGE(M2:M7)</f>
+        <v>8612.5</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="12">
-        <f>SUMIF('[1].xlsx]EJERCICIO-12'!I2:I51,"Prepizzas",'[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>0</v>
+      <c r="M7" s="8">
+        <f>SUMIF($B$2:$B$51,"Prepizza",$F$10:$F$59)</f>
+        <v>6720</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H8" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="12">
-        <f>SUM('[1].xlsx]EJERCICIO-12'!M2:M51)</f>
-        <v>5600</v>
+      <c r="I8" s="12" t="e">
+        <f>SUM(F10:F34)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -993,8 +887,8 @@
         <v>23</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>IF(OR(E16="MERCADO PAGO",E16="TARJETA DE CRÉDITO"),(D16*C16)*$F$2,IF(E16="EFECTIVO",(D16*C16)*$E$3,D16*D16))</f>
+        <v>3240000</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>